<commit_message>
Captura de pantalla y carga en oneDrive
</commit_message>
<xml_diff>
--- a/Prueba_2025/Data/Config.xlsx
+++ b/Prueba_2025/Data/Config.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29231"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D263D86-39A6-4687-9CC5-172CC42C2240}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5249A400-C831-4F2B-B2AB-DCB3C22F2D4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="11">
   <si>
     <t>Key</t>
   </si>
@@ -54,10 +54,7 @@
     <t>ShouldStopMasterAssetName</t>
   </si>
   <si>
-    <t>ExExcelDirectoryPath</t>
-  </si>
-  <si>
-    <t>data_excel</t>
+    <t>sucessFormDirectoryPath</t>
   </si>
 </sst>
 </file>
@@ -469,7 +466,7 @@
         <v>10</v>
       </c>
       <c r="B5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>